<commit_message>
Driver Truck Entry bulk
</commit_message>
<xml_diff>
--- a/static/Account/sampleTruckEntry - Copy.xlsx
+++ b/static/Account/sampleTruckEntry - Copy.xlsx
@@ -496,27 +496,27 @@
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>Custom_Field_2</t>
+          <t>Old Fleet Number</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>Custom_Field_3</t>
+          <t>Old Rego</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>Custom_Field_4</t>
+          <t>Registered Owner</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>Custom_Field_5</t>
+          <t>Roadside Assistance</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>Custom_Field_6</t>
+          <t>PDD number</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">

</xml_diff>